<commit_message>
Añadiendo referencias relativas y absolutas
</commit_message>
<xml_diff>
--- a/Sección04_Paul_Ruiz.xlsx
+++ b/Sección04_Paul_Ruiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAUL\Downloads\Materiales-Para-Descargar\Curso_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{755B2A5B-6741-4220-B06A-8BF40AC885EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56220376-05A6-42E3-88D9-2D94E70E2522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{32CFED9F-5654-4540-A7C3-6568BB8CED3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Parque Infantil</t>
   </si>
@@ -72,29 +72,18 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Enero</t>
-  </si>
-  <si>
-    <t>Febrero</t>
-  </si>
-  <si>
-    <t>Marzo</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Mayo</t>
-  </si>
-  <si>
-    <t>Junio</t>
+    <t>Participación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="mmm\-yyyy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +106,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -135,17 +131,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,130 +464,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8359EC36-ED8C-4451-909D-C5DA7775038E}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.265625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" customWidth="1"/>
+    <col min="7" max="7" width="13.46484375" customWidth="1"/>
+    <col min="8" max="8" width="17.265625" customWidth="1"/>
+    <col min="10" max="10" width="17.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4">
+        <v>43101</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43132</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43160</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43191</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43221</v>
+      </c>
+      <c r="G4" s="4">
+        <v>43252</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>700</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C5" s="2">
+        <v>700</v>
+      </c>
+      <c r="D5" s="2">
+        <v>700</v>
+      </c>
+      <c r="E5" s="2">
+        <v>700</v>
+      </c>
+      <c r="F5" s="2">
+        <v>700</v>
+      </c>
+      <c r="G5" s="2">
+        <v>700</v>
+      </c>
+      <c r="H5" s="2">
+        <f>SUM(B5:G5)</f>
+        <v>4200</v>
+      </c>
+      <c r="J5" s="6">
+        <f>H5/$H$15</f>
+        <v>3.9135296310100633E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
+        <v>4200</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D6" s="2">
         <v>5000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E6" s="2">
+        <v>6000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6000</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" ref="H6:H13" si="0">SUM(B6:G6)</f>
+        <v>29700</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" ref="J6:J13" si="1">H6/$H$15</f>
+        <v>0.27674245247856877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>4300</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C7" s="2">
+        <v>4300</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4300</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4300</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4300</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4300</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>25800</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.24040253447633247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C8" s="2">
+        <v>200</v>
+      </c>
+      <c r="D8" s="2">
+        <v>200</v>
+      </c>
+      <c r="E8" s="2">
+        <v>250</v>
+      </c>
+      <c r="F8" s="2">
+        <v>220</v>
+      </c>
+      <c r="G8" s="2">
+        <v>250</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>1320</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2299664554603056E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>3000</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2300</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3500</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1800</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3000</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>15600</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1453596720089452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="1"/>
+        <v>5.590756615728662E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>5.590756615728662E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>1500</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C12" s="2">
+        <v>1300</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1400</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>9700</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="1"/>
+        <v>9.0383898620946701E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>1500</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>8.386134923592993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <f>SUM(B5:B13)</f>
+        <v>17400</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" ref="C15:G15" si="2">SUM(C5:C13)</f>
+        <v>16500</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="2"/>
+        <v>17500</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="2"/>
+        <v>20250</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="2"/>
+        <v>15920</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>19750</v>
+      </c>
+      <c r="H15" s="2">
+        <f>SUM(B15:G15)</f>
+        <v>107320</v>
+      </c>
+      <c r="J15">
+        <f>SUM(J5:J13)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funcion minimo, maximo, promedio y contar
</commit_message>
<xml_diff>
--- a/Sección04_Paul_Ruiz.xlsx
+++ b/Sección04_Paul_Ruiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAUL\Downloads\Materiales-Para-Descargar\Curso_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B5E1DD-3293-413B-B067-E5F0F0D45CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FAF1D9-7B38-410E-9EA2-E47259682387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{32CFED9F-5654-4540-A7C3-6568BB8CED3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Parque Infantil</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>Participación</t>
+  </si>
+  <si>
+    <t>MÍNIMO</t>
+  </si>
+  <si>
+    <t>MÁXIMO</t>
+  </si>
+  <si>
+    <t>MÁXIMO_6MESES</t>
+  </si>
+  <si>
+    <t>PROMEDIO</t>
+  </si>
+  <si>
+    <t>CONTAR</t>
+  </si>
+  <si>
+    <t>CONTAR_GENERAL</t>
   </si>
 </sst>
 </file>
@@ -467,10 +485,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J15"/>
+  <dimension ref="A2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -810,19 +828,19 @@
         <v>11</v>
       </c>
       <c r="B15" s="2">
-        <f>SUM(B5:B13)</f>
+        <f>SUM(B5:B14)</f>
         <v>17400</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" ref="C15:G15" si="2">SUM(C5:C13)</f>
+        <f>SUM(C5:C13)</f>
         <v>16500</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="2"/>
+        <f>SUM(D5:D13)</f>
         <v>17500</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E15:H15" si="2">SUM(E5:E13)</f>
         <v>20250</v>
       </c>
       <c r="F15" s="2">
@@ -834,12 +852,146 @@
         <v>19750</v>
       </c>
       <c r="H15" s="2">
-        <f>SUM(B15:G15)</f>
+        <f t="shared" si="2"/>
         <v>107320</v>
       </c>
       <c r="J15">
         <f>SUM(J5:J13)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <f>MIN(B5:B13)</f>
+        <v>200</v>
+      </c>
+      <c r="C17" s="2">
+        <f>MIN(C5:C13)</f>
+        <v>200</v>
+      </c>
+      <c r="D17" s="2">
+        <f>MIN(D5:D13)</f>
+        <v>200</v>
+      </c>
+      <c r="E17" s="2">
+        <f>MIN(E5:E13)</f>
+        <v>250</v>
+      </c>
+      <c r="F17" s="2">
+        <f>MIN(F5:F13)</f>
+        <v>220</v>
+      </c>
+      <c r="G17" s="2">
+        <f>MIN(G5:G13)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2">
+        <f>MAX(B5:B13)</f>
+        <v>4300</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:G18" si="3">MAX(C5:C13)</f>
+        <v>4500</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="3"/>
+        <v>4300</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2">
+        <f>MAX(B5:G13)</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2">
+        <f>AVERAGE(B5:B13)</f>
+        <v>1933.3333333333333</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" ref="C20:G20" si="4">AVERAGE(C5:C13)</f>
+        <v>1833.3333333333333</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="4"/>
+        <v>1944.4444444444443</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="4"/>
+        <v>2250</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="4"/>
+        <v>1768.8888888888889</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="4"/>
+        <v>2194.4444444444443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <f>COUNT(B5:B13)</f>
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:G21" si="5">COUNT(C5:C13)</f>
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <f>COUNT(B5:G13)</f>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalizando la seccion 05
</commit_message>
<xml_diff>
--- a/Sección04_Paul_Ruiz.xlsx
+++ b/Sección04_Paul_Ruiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAUL\Downloads\Materiales-Para-Descargar\Curso_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FAF1D9-7B38-410E-9EA2-E47259682387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF48353A-7F93-4070-9B2A-475B01C0FF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{32CFED9F-5654-4540-A7C3-6568BB8CED3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Parque Infantil</t>
   </si>
@@ -70,6 +70,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
   </si>
   <si>
     <t>Participación</t>
@@ -99,7 +117,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -159,14 +177,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +503,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J22"/>
+  <dimension ref="A2:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -505,43 +523,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>43101</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>43132</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>43160</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>43191</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>43221</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>43252</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -570,7 +588,7 @@
         <f>SUM(B5:G5)</f>
         <v>4200</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <f>H5/$H$15</f>
         <v>3.9135296310100633E-2</v>
       </c>
@@ -601,7 +619,7 @@
         <f t="shared" ref="H6:H13" si="0">SUM(B6:G6)</f>
         <v>29700</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f t="shared" ref="J6:J13" si="1">H6/$H$15</f>
         <v>0.27674245247856877</v>
       </c>
@@ -632,7 +650,7 @@
         <f t="shared" si="0"/>
         <v>25800</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <f t="shared" si="1"/>
         <v>0.24040253447633247</v>
       </c>
@@ -663,7 +681,7 @@
         <f t="shared" si="0"/>
         <v>1320</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <f t="shared" si="1"/>
         <v>1.2299664554603056E-2</v>
       </c>
@@ -694,7 +712,7 @@
         <f t="shared" si="0"/>
         <v>15600</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <f t="shared" si="1"/>
         <v>0.1453596720089452</v>
       </c>
@@ -725,7 +743,7 @@
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <f t="shared" si="1"/>
         <v>5.590756615728662E-2</v>
       </c>
@@ -756,7 +774,7 @@
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <f t="shared" si="1"/>
         <v>5.590756615728662E-2</v>
       </c>
@@ -787,7 +805,7 @@
         <f t="shared" si="0"/>
         <v>9700</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <f t="shared" si="1"/>
         <v>9.0383898620946701E-2</v>
       </c>
@@ -818,7 +836,7 @@
         <f t="shared" si="0"/>
         <v>9000</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <f t="shared" si="1"/>
         <v>8.386134923592993E-2</v>
       </c>
@@ -832,15 +850,15 @@
         <v>17400</v>
       </c>
       <c r="C15" s="2">
-        <f>SUM(C5:C13)</f>
+        <f t="shared" ref="C15:G15" si="2">SUM(C5:C14)</f>
         <v>16500</v>
       </c>
       <c r="D15" s="2">
-        <f>SUM(D5:D13)</f>
+        <f t="shared" si="2"/>
         <v>17500</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:H15" si="2">SUM(E5:E13)</f>
+        <f t="shared" si="2"/>
         <v>20250</v>
       </c>
       <c r="F15" s="2">
@@ -852,7 +870,7 @@
         <v>19750</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="2"/>
+        <f>SUM(H5:H14)</f>
         <v>107320</v>
       </c>
       <c r="J15">
@@ -860,138 +878,218 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
-        <f>MIN(B5:B13)</f>
+        <f t="shared" ref="B17:G17" si="3">MIN(B5:B13)</f>
         <v>200</v>
       </c>
       <c r="C17" s="2">
-        <f>MIN(C5:C13)</f>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="D17" s="2">
-        <f>MIN(D5:D13)</f>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="E17" s="2">
-        <f>MIN(E5:E13)</f>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="F17" s="2">
-        <f>MIN(F5:F13)</f>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="G17" s="2">
-        <f>MIN(G5:G13)</f>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <f>MAX(B5:B13)</f>
         <v>4300</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:G18" si="3">MAX(C5:C13)</f>
+        <f t="shared" ref="C18:G18" si="4">MAX(C5:C13)</f>
         <v>4500</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6000</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4300</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <f>MAX(B5:G13)</f>
         <v>6000</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
         <f>AVERAGE(B5:B13)</f>
         <v>1933.3333333333333</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" ref="C20:G20" si="4">AVERAGE(C5:C13)</f>
+        <f t="shared" ref="C20:G20" si="5">AVERAGE(C5:C13)</f>
         <v>1833.3333333333333</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1944.4444444444443</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2250</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1768.8888888888889</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2194.4444444444443</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <f>COUNT(B5:B13)</f>
         <v>9</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:G21" si="5">COUNT(C5:C13)</f>
+        <f t="shared" ref="C21:G21" si="6">COUNT(C5:C13)</f>
         <v>9</v>
       </c>
       <c r="D21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="E21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="F21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <f>COUNT(B5:G13)</f>
         <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F35">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>